<commit_message>
newest ac dimer + convolved pulse lineshape fit code
</commit_message>
<xml_diff>
--- a/clockshift/metadata_dimer_file.xlsx
+++ b/clockshift/metadata_dimer_file.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/clockshift/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC0852-C93C-4F4A-B8AF-C7508DF9DEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186D3ED-1042-0D40-BF7F-3E0965589DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16720" xr2:uid="{4C901807-9D65-8B46-8461-7DE462309F00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>filename</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>2024-08-12_L_e</t>
+  </si>
+  <si>
+    <t>2024-09-27_B_e</t>
+  </si>
+  <si>
+    <t>2024-09-27_C_e</t>
   </si>
 </sst>
 </file>
@@ -494,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A312CE99-8F9F-FA49-B765-C08DBFD6DDE4}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -944,8 +950,8 @@
       <c r="G10">
         <v>1.8</v>
       </c>
-      <c r="H10">
-        <v>-3.95</v>
+      <c r="H10" s="1">
+        <v>-3.96</v>
       </c>
       <c r="I10">
         <v>-3.9</v>
@@ -991,8 +997,8 @@
       <c r="G11">
         <v>2.0499999999999998</v>
       </c>
-      <c r="H11">
-        <v>-3.95</v>
+      <c r="H11" s="1">
+        <v>-3.96</v>
       </c>
       <c r="I11">
         <v>-3.9</v>
@@ -1039,7 +1045,7 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="H12" s="1">
-        <v>-3.95</v>
+        <v>-3.96</v>
       </c>
       <c r="I12" s="1">
         <v>-3.9</v>
@@ -1087,7 +1093,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="1">
-        <v>-3.95</v>
+        <v>-3.96</v>
       </c>
       <c r="I13" s="1">
         <v>-3.9</v>
@@ -1135,7 +1141,7 @@
         <v>4.5</v>
       </c>
       <c r="H14" s="1">
-        <v>-3.95</v>
+        <v>-3.96</v>
       </c>
       <c r="I14" s="1">
         <v>-3.9</v>
@@ -1205,6 +1211,94 @@
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="I16" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="J16" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="K16" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+      <c r="P16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>18.2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="H17" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="J17" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="K17" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+      <c r="P17" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit recent -- dimer and sum rule
</commit_message>
<xml_diff>
--- a/clockshift/metadata_dimer_file.xlsx
+++ b/clockshift/metadata_dimer_file.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/clockshift/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Analysis Scripts\analysis\clockshift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A186D3ED-1042-0D40-BF7F-3E0965589DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16720" xr2:uid="{4C901807-9D65-8B46-8461-7DE462309F00}"/>
+    <workbookView xWindow="0" yWindow="735" windowWidth="29400" windowHeight="16725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t>filename</t>
   </si>
@@ -141,13 +140,64 @@
   </si>
   <si>
     <t>2024-09-27_C_e</t>
+  </si>
+  <si>
+    <t>2024-10-01_F_e</t>
+  </si>
+  <si>
+    <t>2024-10-02_C_e</t>
+  </si>
+  <si>
+    <t>barnu</t>
+  </si>
+  <si>
+    <t>2024-10-03_C_e</t>
+  </si>
+  <si>
+    <t>EF2</t>
+  </si>
+  <si>
+    <t>ToTF2</t>
+  </si>
+  <si>
+    <t>trackbg</t>
+  </si>
+  <si>
+    <t>2024-10-04_H_e</t>
+  </si>
+  <si>
+    <t>2024-10-07_C_e</t>
+  </si>
+  <si>
+    <t>2024-10-07_G_e</t>
+  </si>
+  <si>
+    <t>[[0,6],[10,15]]</t>
+  </si>
+  <si>
+    <t>bg_freq</t>
+  </si>
+  <si>
+    <t>[[-3.96, -3.9]]</t>
+  </si>
+  <si>
+    <t>[[-3.7, -3.6]]</t>
+  </si>
+  <si>
+    <t>[[-5.1, -4.9]]</t>
+  </si>
+  <si>
+    <t>2024-10-10_D_e</t>
+  </si>
+  <si>
+    <t>[[-5.1, -4.9],[-3.1,-2.9]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +211,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,9 +239,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,19 +556,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A312CE99-8F9F-FA49-B765-C08DBFD6DDE4}">
-  <dimension ref="A1:P17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="5.375" customWidth="1"/>
+    <col min="4" max="4" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,43 +584,58 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -575,37 +649,43 @@
         <v>6.4000000000000005E-4</v>
       </c>
       <c r="E2">
+        <v>352</v>
+      </c>
+      <c r="F2">
         <v>15.2</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>0.31</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>1.4</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>-3.96</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>-3.9</v>
       </c>
-      <c r="J2">
-        <v>202.14</v>
-      </c>
-      <c r="K2">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2">
+        <v>202.14</v>
+      </c>
+      <c r="O2">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P2" t="s">
         <v>16</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -619,37 +699,43 @@
         <v>6.4000000000000005E-4</v>
       </c>
       <c r="E3">
+        <v>352</v>
+      </c>
+      <c r="F3">
         <v>13.3</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.34</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <v>1.5</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>-3.96</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>-3.9</v>
       </c>
-      <c r="J3">
-        <v>202.14</v>
-      </c>
-      <c r="K3">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3">
+        <v>202.14</v>
+      </c>
+      <c r="O3">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -663,37 +749,43 @@
         <v>6.4000000000000005E-4</v>
       </c>
       <c r="E4">
+        <v>352</v>
+      </c>
+      <c r="F4">
         <v>13.3</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.34</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <v>1.45</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>-3.96</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>-3.9</v>
       </c>
-      <c r="J4">
-        <v>202.14</v>
-      </c>
-      <c r="K4">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="M4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4">
+        <v>202.14</v>
+      </c>
+      <c r="O4">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P4" t="s">
         <v>16</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -707,40 +799,46 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E5">
+        <v>352</v>
+      </c>
+      <c r="F5">
         <v>14</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.315</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>1.8</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>-3.95</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>-3.9</v>
       </c>
-      <c r="J5">
-        <v>202.14</v>
-      </c>
-      <c r="K5">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="M5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5">
+        <v>202.14</v>
+      </c>
+      <c r="O5">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P5" t="s">
         <v>16</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>0.33</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -754,40 +852,46 @@
         <v>1.6000000000000001E-4</v>
       </c>
       <c r="E6">
+        <v>352</v>
+      </c>
+      <c r="F6">
         <v>11.5</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.315</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>8</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>-3.95</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>-3.9</v>
       </c>
-      <c r="J6">
-        <v>202.14</v>
-      </c>
-      <c r="K6">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="M6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6">
+        <v>202.14</v>
+      </c>
+      <c r="O6">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P6" t="s">
         <v>21</v>
       </c>
-      <c r="M6">
+      <c r="Q6">
         <v>0.2</v>
       </c>
-      <c r="N6">
+      <c r="R6">
         <v>0.55200000000000005</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -801,40 +905,46 @@
         <v>1.6000000000000001E-4</v>
       </c>
       <c r="E7">
+        <v>352</v>
+      </c>
+      <c r="F7">
         <v>14</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.315</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>7</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>-3.95</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>-3.9</v>
       </c>
-      <c r="J7">
-        <v>202.14</v>
-      </c>
-      <c r="K7">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7">
+        <v>202.14</v>
+      </c>
+      <c r="O7">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P7" t="s">
         <v>21</v>
       </c>
-      <c r="M7">
+      <c r="Q7">
         <v>0.2</v>
       </c>
-      <c r="O7">
+      <c r="S7">
         <v>17</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -848,40 +958,46 @@
         <v>1.6000000000000001E-4</v>
       </c>
       <c r="E8">
+        <v>352</v>
+      </c>
+      <c r="F8">
         <v>12.1</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.29699999999999999</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>5</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>-3.95</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>-3.9</v>
       </c>
-      <c r="J8">
-        <v>202.14</v>
-      </c>
-      <c r="K8">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="M8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N8">
+        <v>202.14</v>
+      </c>
+      <c r="O8">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P8" t="s">
         <v>21</v>
       </c>
-      <c r="M8">
+      <c r="Q8">
         <v>0.2</v>
       </c>
-      <c r="N8">
+      <c r="R8">
         <v>0.35199999999999998</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -895,40 +1011,46 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E9">
+        <v>352</v>
+      </c>
+      <c r="F9">
         <v>12.1</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>0.29699999999999999</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>6.5</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>-3.95</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>-3.9</v>
       </c>
-      <c r="J9">
-        <v>202.14</v>
-      </c>
-      <c r="K9">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="M9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N9">
+        <v>202.14</v>
+      </c>
+      <c r="O9">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P9" t="s">
         <v>21</v>
       </c>
-      <c r="M9">
+      <c r="Q9">
         <v>0.2</v>
       </c>
-      <c r="N9">
+      <c r="R9">
         <v>0.42799999999999999</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -942,40 +1064,46 @@
         <v>8.0000000000000007E-5</v>
       </c>
       <c r="E10">
+        <v>352</v>
+      </c>
+      <c r="F10">
         <v>11.85</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>0.41649999999999998</v>
       </c>
-      <c r="G10">
+      <c r="J10">
         <v>1.8</v>
       </c>
-      <c r="H10" s="1">
+      <c r="K10" s="1">
         <v>-3.96</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>-3.9</v>
       </c>
-      <c r="J10">
-        <v>202.14</v>
-      </c>
-      <c r="K10">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="M10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10">
+        <v>202.14</v>
+      </c>
+      <c r="O10">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P10" t="s">
         <v>16</v>
       </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
         <v>0.35</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -989,40 +1117,46 @@
         <v>4.0000000000000003E-5</v>
       </c>
       <c r="E11">
+        <v>352</v>
+      </c>
+      <c r="F11">
         <v>11.85</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>0.41649999999999998</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <v>2.0499999999999998</v>
       </c>
-      <c r="H11" s="1">
+      <c r="K11" s="1">
         <v>-3.96</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>-3.9</v>
       </c>
-      <c r="J11">
-        <v>202.14</v>
-      </c>
-      <c r="K11">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="M11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11">
+        <v>202.14</v>
+      </c>
+      <c r="O11">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P11" t="s">
         <v>16</v>
       </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
         <v>0.49199999999999999</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="U11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1035,42 +1169,50 @@
       <c r="D12" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
+        <v>352</v>
+      </c>
+      <c r="F12" s="1">
         <v>11.85</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="1"/>
+      <c r="H12">
         <v>0.41649999999999998</v>
       </c>
-      <c r="G12" s="1">
+      <c r="J12" s="1">
         <v>2.3199999999999998</v>
       </c>
-      <c r="H12" s="1">
+      <c r="K12" s="1">
         <v>-3.96</v>
       </c>
-      <c r="I12" s="1">
+      <c r="L12" s="1">
         <v>-3.9</v>
       </c>
-      <c r="J12" s="1">
-        <v>202.14</v>
-      </c>
-      <c r="K12" s="1">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O12" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="1">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1">
+      <c r="Q12" s="1">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1">
         <v>0.66</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1083,42 +1225,50 @@
       <c r="D13" s="1">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
+        <v>352</v>
+      </c>
+      <c r="F13" s="1">
         <v>11.85</v>
       </c>
-      <c r="F13">
+      <c r="G13" s="1"/>
+      <c r="H13">
         <v>0.41649999999999998</v>
       </c>
-      <c r="G13" s="1">
+      <c r="J13" s="1">
         <v>7</v>
       </c>
-      <c r="H13" s="1">
+      <c r="K13" s="1">
         <v>-3.96</v>
       </c>
-      <c r="I13" s="1">
+      <c r="L13" s="1">
         <v>-3.9</v>
       </c>
-      <c r="J13" s="1">
-        <v>202.14</v>
-      </c>
-      <c r="K13" s="1">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O13" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="1">
+      <c r="Q13" s="1">
         <v>0.5</v>
       </c>
-      <c r="N13" s="1">
+      <c r="R13" s="1">
         <v>1.18</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1131,42 +1281,50 @@
       <c r="D14" s="1">
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
+        <v>352</v>
+      </c>
+      <c r="F14" s="1">
         <v>11.85</v>
       </c>
-      <c r="F14">
+      <c r="G14" s="1"/>
+      <c r="H14">
         <v>0.41649999999999998</v>
       </c>
-      <c r="G14" s="1">
+      <c r="J14" s="1">
         <v>4.5</v>
       </c>
-      <c r="H14" s="1">
+      <c r="K14" s="1">
         <v>-3.96</v>
       </c>
-      <c r="I14" s="1">
+      <c r="L14" s="1">
         <v>-3.9</v>
       </c>
-      <c r="J14" s="1">
-        <v>202.14</v>
-      </c>
-      <c r="K14" s="1">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O14" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="1">
+      <c r="Q14" s="1">
         <v>0.5</v>
       </c>
-      <c r="N14" s="1">
+      <c r="R14" s="1">
         <v>0.71599999999999997</v>
       </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1179,42 +1337,50 @@
       <c r="D15" s="1">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
+        <v>352</v>
+      </c>
+      <c r="F15" s="1">
         <v>12</v>
       </c>
-      <c r="F15">
+      <c r="G15" s="1"/>
+      <c r="H15">
         <v>0.39900000000000002</v>
       </c>
-      <c r="G15" s="1">
+      <c r="J15" s="1">
         <v>4.5</v>
       </c>
-      <c r="H15" s="1">
+      <c r="K15" s="1">
         <v>-3.7</v>
       </c>
-      <c r="I15" s="1">
+      <c r="L15" s="1">
         <v>-3.6</v>
       </c>
-      <c r="J15" s="1">
-        <v>202.14</v>
-      </c>
-      <c r="K15" s="1">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N15" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O15" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="1">
+      <c r="Q15" s="1">
         <v>0.5</v>
       </c>
-      <c r="N15" s="1">
+      <c r="R15" s="1">
         <v>0.71599999999999997</v>
       </c>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1228,37 +1394,51 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="E16" s="1">
+        <v>377</v>
+      </c>
+      <c r="F16" s="1">
         <v>18.2</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1">
         <v>0.53700000000000003</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
         <v>5</v>
       </c>
-      <c r="H16" s="1">
+      <c r="K16" s="1">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="I16" s="1">
+      <c r="L16" s="1">
         <v>-4.9000000000000004</v>
       </c>
-      <c r="J16" s="1">
-        <v>202.14</v>
-      </c>
-      <c r="K16" s="1">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O16" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M16" s="1">
-        <v>1</v>
-      </c>
-      <c r="P16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
+        <v>45</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1272,37 +1452,438 @@
         <v>2.0000000000000002E-5</v>
       </c>
       <c r="E17" s="1">
+        <v>377</v>
+      </c>
+      <c r="F17" s="1">
         <v>18.2</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
         <v>0.53700000000000003</v>
       </c>
-      <c r="G17" s="1">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1">
         <v>3.5</v>
       </c>
-      <c r="H17" s="1">
+      <c r="K17" s="1">
         <v>-5.0999999999999996</v>
       </c>
-      <c r="I17" s="1">
+      <c r="L17" s="1">
         <v>-4.9000000000000004</v>
       </c>
-      <c r="J17" s="1">
-        <v>202.14</v>
-      </c>
-      <c r="K17" s="1">
-        <v>47.222700000000003</v>
-      </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O17" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="1">
-        <v>1</v>
-      </c>
-      <c r="P17" s="1">
+      <c r="Q17" s="1">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="U17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E18" s="1">
+        <v>377</v>
+      </c>
+      <c r="F18" s="2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="1">
+        <v>0.439</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1">
+        <v>4</v>
+      </c>
+      <c r="K18" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L18" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O18" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E19" s="1">
+        <v>377</v>
+      </c>
+      <c r="F19" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L19" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O19" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>377</v>
+      </c>
+      <c r="F20" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="G20" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="J20" s="1">
+        <v>4</v>
+      </c>
+      <c r="K20" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L20" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O20" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>1</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>377</v>
+      </c>
+      <c r="F21" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1">
+        <v>0.442</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L21" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O21" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>1</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>377</v>
+      </c>
+      <c r="F22" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="J22" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="K22" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L22" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N22" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O22" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>377</v>
+      </c>
+      <c r="F23" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="J23" s="1">
+        <v>5</v>
+      </c>
+      <c r="K23" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L23" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O23" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>1</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>377</v>
+      </c>
+      <c r="F24" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="G24" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="J24" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="K24" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L24" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N24" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O24" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
analysis fixes and some small box tests
</commit_message>
<xml_diff>
--- a/clockshift/metadata_dimer_file.xlsx
+++ b/clockshift/metadata_dimer_file.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Analysis Scripts\analysis\clockshift\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinxie/Documents/GitHub/analysis/clockshift/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B997A5D6-9E32-6341-A011-E7B61BD0A272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="29400" windowHeight="16725"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="56">
   <si>
     <t>filename</t>
   </si>
@@ -160,9 +150,6 @@
     <t>ToTF2</t>
   </si>
   <si>
-    <t>trackbg</t>
-  </si>
-  <si>
     <t>2024-10-04_H_e</t>
   </si>
   <si>
@@ -191,12 +178,27 @@
   </si>
   <si>
     <t>[[-5.1, -4.9],[-3.1,-2.9]]</t>
+  </si>
+  <si>
+    <t>[[-4.1, -4.04],[-3.96, -3.9]]</t>
+  </si>
+  <si>
+    <t>load_lineshape</t>
+  </si>
+  <si>
+    <t>track_bg</t>
+  </si>
+  <si>
+    <t>2024-10-02_C_e_smallbox</t>
+  </si>
+  <si>
+    <t>2024-10-03_C_e_smallbox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -556,21 +558,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.875" customWidth="1"/>
-    <col min="3" max="3" width="5.375" customWidth="1"/>
-    <col min="4" max="4" width="9.25" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" t="s">
         <v>7</v>
@@ -629,13 +631,16 @@
         <v>10</v>
       </c>
       <c r="T1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="U1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -667,7 +672,7 @@
         <v>-3.9</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N2">
         <v>202.14</v>
@@ -681,11 +686,17 @@
       <c r="Q2">
         <v>1</v>
       </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
       <c r="U2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -717,7 +728,7 @@
         <v>-3.9</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N3">
         <v>202.14</v>
@@ -731,11 +742,17 @@
       <c r="Q3">
         <v>1</v>
       </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
       <c r="U3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -767,7 +784,7 @@
         <v>-3.9</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N4">
         <v>202.14</v>
@@ -781,11 +798,17 @@
       <c r="Q4">
         <v>1</v>
       </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
       <c r="U4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -817,7 +840,7 @@
         <v>-3.9</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N5">
         <v>202.14</v>
@@ -834,11 +857,17 @@
       <c r="R5">
         <v>0.33</v>
       </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
       <c r="U5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -870,7 +899,7 @@
         <v>-3.9</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N6">
         <v>202.14</v>
@@ -887,11 +916,17 @@
       <c r="R6">
         <v>0.55200000000000005</v>
       </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
       <c r="U6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -923,7 +958,7 @@
         <v>-3.9</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N7">
         <v>202.14</v>
@@ -940,11 +975,17 @@
       <c r="S7">
         <v>17</v>
       </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
       <c r="U7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -976,7 +1017,7 @@
         <v>-3.9</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N8">
         <v>202.14</v>
@@ -993,11 +1034,17 @@
       <c r="R8">
         <v>0.35199999999999998</v>
       </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
       <c r="U8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1029,7 +1076,7 @@
         <v>-3.9</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N9">
         <v>202.14</v>
@@ -1046,11 +1093,17 @@
       <c r="R9">
         <v>0.42799999999999999</v>
       </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
       <c r="U9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1082,7 +1135,7 @@
         <v>-3.9</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N10">
         <v>202.14</v>
@@ -1099,11 +1152,17 @@
       <c r="R10">
         <v>0.35</v>
       </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
       <c r="U10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1135,7 +1194,7 @@
         <v>-3.9</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N11">
         <v>202.14</v>
@@ -1152,11 +1211,17 @@
       <c r="R11">
         <v>0.49199999999999999</v>
       </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
       <c r="U11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1189,7 +1254,7 @@
         <v>-3.9</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N12" s="1">
         <v>202.14</v>
@@ -1207,12 +1272,17 @@
         <v>0.66</v>
       </c>
       <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -1245,7 +1315,7 @@
         <v>-3.9</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N13" s="1">
         <v>202.14</v>
@@ -1263,12 +1333,17 @@
         <v>1.18</v>
       </c>
       <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>30</v>
       </c>
@@ -1301,7 +1376,7 @@
         <v>-3.9</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N14" s="1">
         <v>202.14</v>
@@ -1319,12 +1394,17 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -1357,7 +1437,7 @@
         <v>-3.6</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N15" s="1">
         <v>202.14</v>
@@ -1375,12 +1455,17 @@
         <v>0.71599999999999997</v>
       </c>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
@@ -1414,7 +1499,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N16" s="1">
         <v>202.14</v>
@@ -1429,16 +1514,19 @@
         <v>1</v>
       </c>
       <c r="S16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T16">
         <v>1</v>
       </c>
-      <c r="U16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>1</v>
+      </c>
+      <c r="V16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -1472,7 +1560,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N17" s="1">
         <v>202.14</v>
@@ -1489,11 +1577,14 @@
       <c r="T17">
         <v>1</v>
       </c>
-      <c r="U17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1618,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N18" s="1">
         <v>202.14</v>
@@ -1544,11 +1635,14 @@
       <c r="T18">
         <v>1</v>
       </c>
-      <c r="U18" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1582,7 +1676,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N19" s="1">
         <v>202.14</v>
@@ -1599,11 +1693,14 @@
       <c r="T19">
         <v>1</v>
       </c>
-      <c r="U19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1641,7 +1738,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N20" s="1">
         <v>202.14</v>
@@ -1658,13 +1755,16 @@
       <c r="T20">
         <v>1</v>
       </c>
-      <c r="U20" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -1696,7 +1796,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N21" s="1">
         <v>202.14</v>
@@ -1713,13 +1813,16 @@
       <c r="T21">
         <v>1</v>
       </c>
-      <c r="U21" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
@@ -1749,7 +1852,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N22" s="1">
         <v>202.14</v>
@@ -1766,13 +1869,16 @@
       <c r="T22">
         <v>1</v>
       </c>
-      <c r="U22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
@@ -1802,7 +1908,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N23" s="1">
         <v>202.14</v>
@@ -1819,13 +1925,16 @@
       <c r="T23">
         <v>1</v>
       </c>
-      <c r="U23" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>1</v>
+      </c>
+      <c r="V23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
@@ -1861,7 +1970,7 @@
         <v>-4.9000000000000004</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N24" s="1">
         <v>202.14</v>
@@ -1878,7 +1987,130 @@
       <c r="T24">
         <v>1</v>
       </c>
-      <c r="U24" s="1">
+      <c r="U24">
+        <v>1</v>
+      </c>
+      <c r="V24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>377</v>
+      </c>
+      <c r="F25" s="1">
+        <v>15.1</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <v>4</v>
+      </c>
+      <c r="K25" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L25" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N25" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O25" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>1</v>
+      </c>
+      <c r="V25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>377</v>
+      </c>
+      <c r="F26" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>14.1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="J26" s="1">
+        <v>4</v>
+      </c>
+      <c r="K26" s="1">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="L26" s="1">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N26" s="1">
+        <v>202.14</v>
+      </c>
+      <c r="O26" s="1">
+        <v>47.222700000000003</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>